<commit_message>
corrections in graphs; new analysis short-term AmE, with 3 macro genres
</commit_message>
<xml_diff>
--- a/data/excel/Historical_collections_fool.xlsx
+++ b/data/excel/Historical_collections_fool.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ba4es16\Work Folders\Documents\Aufsätze\Leuven 2022\R_project_verbs_of_deceiving\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\daten.uni-bamberg.de\Aufgabenbezogen_M\eng-ling\Deceive-type verbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6767" uniqueCount="2140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6827" uniqueCount="2156">
   <si>
     <t>y</t>
   </si>
@@ -6447,6 +6447,54 @@
   </si>
   <si>
     <t>verbal</t>
+  </si>
+  <si>
+    <t>So that's very, very important because it can be very misleading and you could be</t>
+  </si>
+  <si>
+    <t>that there's nothing wrong with the baby, then there'll also be swelling of the hands, feet and the eyelids might swell up, the medical word for that is oedema which you may well see in books, which means swelling [pause] occasionally the overlying skin is</t>
+  </si>
+  <si>
+    <t>It was also discovered that egg production could be boosted by leaving lights on in the houses all night to</t>
+  </si>
+  <si>
+    <t>fool the hens into thinking</t>
+  </si>
+  <si>
+    <t>that it was still daylight.</t>
+  </si>
+  <si>
+    <t>A lot of people (.) a lot of new parents yes (.) they are</t>
+  </si>
+  <si>
+    <t>that they must listen to their children and respect their</t>
+  </si>
+  <si>
+    <t>ah (.) he 's interested in slight of hand S0173: yeah (.) if he can</t>
+  </si>
+  <si>
+    <t>fool people into you know believing</t>
+  </si>
+  <si>
+    <t>a coin has been passed to another</t>
+  </si>
+  <si>
+    <t>and like redeploy like different areas to</t>
+  </si>
+  <si>
+    <t>fool one person into thinking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">that it 's round S0544: &gt;&gt;worth worth </t>
+  </si>
+  <si>
+    <t>BNC2014</t>
+  </si>
+  <si>
+    <t>BNC2015</t>
+  </si>
+  <si>
+    <t>BNC2016</t>
   </si>
 </sst>
 </file>
@@ -6791,12 +6839,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB423"/>
+  <dimension ref="A1:AB428"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A416" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A415" sqref="A415:XFD415"/>
+      <selection pane="bottomLeft" activeCell="K426" sqref="K426:N428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34155,6 +34203,211 @@
       </c>
       <c r="M423" s="5"/>
     </row>
+    <row r="424" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A424" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C424" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="E424" s="5">
+        <v>1993</v>
+      </c>
+      <c r="F424" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G424" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H424" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I424" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="J424" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L424" s="4" t="s">
+        <v>2140</v>
+      </c>
+      <c r="M424" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="N424" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="425" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A425" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C425" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="E425" s="5">
+        <v>1994</v>
+      </c>
+      <c r="F425" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G425" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H425" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I425" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="J425" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L425" s="4" t="s">
+        <v>2142</v>
+      </c>
+      <c r="M425" s="4" t="s">
+        <v>2143</v>
+      </c>
+      <c r="N425" t="s">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="426" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A426" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C426" s="2" t="s">
+        <v>2153</v>
+      </c>
+      <c r="D426" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="E426" s="5">
+        <v>2012</v>
+      </c>
+      <c r="F426" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G426" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H426" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I426" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="J426" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L426" s="4" t="s">
+        <v>2145</v>
+      </c>
+      <c r="M426" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="N426" t="s">
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="427" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A427" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C427" s="2" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="E427" s="5">
+        <v>2012</v>
+      </c>
+      <c r="F427" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G427" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H427" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I427" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="J427" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L427" s="4" t="s">
+        <v>2147</v>
+      </c>
+      <c r="M427" s="1" t="s">
+        <v>2148</v>
+      </c>
+      <c r="N427" t="s">
+        <v>2149</v>
+      </c>
+    </row>
+    <row r="428" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A428" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C428" s="2" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="E428" s="5">
+        <v>2016</v>
+      </c>
+      <c r="F428" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G428" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H428" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I428" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="J428" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L428" s="4" t="s">
+        <v>2150</v>
+      </c>
+      <c r="M428" s="4" t="s">
+        <v>2151</v>
+      </c>
+      <c r="N428" s="1" t="s">
+        <v>2152</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB376"/>
   <sortState ref="A2:AB405">

</xml_diff>